<commit_message>
Modifiche e correzioni minori
Corretti alcuni errori di battitura ecc.
</commit_message>
<xml_diff>
--- a/Parte 3/Esercizio 2/dati.xlsx
+++ b/Parte 3/Esercizio 2/dati.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -69,15 +69,6 @@
     <t>FATTURATO CON PREVISIONE (GRAFICO)</t>
   </si>
   <si>
-    <t>facendo la media stagionale</t>
-  </si>
-  <si>
-    <t>dividendo i valor con media annuale</t>
-  </si>
-  <si>
-    <t>dividendo i valori sopra con indice stagionale</t>
-  </si>
-  <si>
     <t>fatturato destagionalizzato</t>
   </si>
   <si>
@@ -86,11 +77,20 @@
   <si>
     <t xml:space="preserve">usando la retta di interpolazione del </t>
   </si>
+  <si>
+    <t>calcolando la media stagionale</t>
+  </si>
+  <si>
+    <t>dividendo i valori con la media annuale</t>
+  </si>
+  <si>
+    <t>dividendo i valori sopra con l'indice stagionale</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -181,12 +181,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -195,6 +189,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -214,7 +214,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="it-IT"/>
   <c:roundedCorners val="0"/>
@@ -432,7 +432,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-561E-48ED-BA15-F80349ABA6E9}"/>
             </c:ext>
@@ -448,11 +448,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="858192287"/>
-        <c:axId val="858191455"/>
+        <c:axId val="151436072"/>
+        <c:axId val="151429800"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="858192287"/>
+        <c:axId val="151436072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -495,7 +495,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="858191455"/>
+        <c:crossAx val="151429800"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -503,7 +503,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="858191455"/>
+        <c:axId val="151429800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -554,7 +554,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="858192287"/>
+        <c:crossAx val="151436072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -604,7 +604,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="it-IT"/>
   <c:roundedCorners val="0"/>
@@ -835,7 +835,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-B86C-4055-8C6B-1B0C2886FD54}"/>
             </c:ext>
@@ -851,11 +851,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="858192287"/>
-        <c:axId val="858191455"/>
+        <c:axId val="151432152"/>
+        <c:axId val="151432544"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="858192287"/>
+        <c:axId val="151432152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -898,7 +898,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="858191455"/>
+        <c:crossAx val="151432544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -906,7 +906,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="858191455"/>
+        <c:axId val="151432544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="30"/>
@@ -958,7 +958,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="858192287"/>
+        <c:crossAx val="151432152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1008,7 +1008,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="it-IT"/>
   <c:roundedCorners val="0"/>
@@ -1250,7 +1250,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-3BE2-487E-AA63-AB62D18CD03F}"/>
             </c:ext>
@@ -1266,11 +1266,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="1485811376"/>
-        <c:axId val="1485807632"/>
+        <c:axId val="151434112"/>
+        <c:axId val="381669952"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1485811376"/>
+        <c:axId val="151434112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1313,7 +1313,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1485807632"/>
+        <c:crossAx val="381669952"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1321,7 +1321,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1485807632"/>
+        <c:axId val="381669952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1372,7 +1372,7 @@
             <a:endParaRPr lang="it-IT"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1485811376"/>
+        <c:crossAx val="151434112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3412,33 +3412,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:V52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="D10" workbookViewId="0">
+      <selection activeCell="H20" sqref="H20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="2" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B2" s="10" t="s">
+    <row r="2" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B2" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="K2" s="10" t="s">
+      <c r="C2" s="13"/>
+      <c r="D2" s="13"/>
+      <c r="E2" s="13"/>
+      <c r="F2" s="13"/>
+      <c r="G2" s="13"/>
+      <c r="K2" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="10"/>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="10"/>
-      <c r="R2" s="10"/>
+      <c r="L2" s="13"/>
+      <c r="M2" s="13"/>
+      <c r="N2" s="13"/>
+      <c r="O2" s="13"/>
+      <c r="P2" s="13"/>
+      <c r="Q2" s="13"/>
+      <c r="R2" s="13"/>
     </row>
-    <row r="3" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
@@ -3482,7 +3482,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B4" s="2">
         <v>1</v>
       </c>
@@ -3527,7 +3527,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="5" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B5" s="2">
         <v>2</v>
       </c>
@@ -3548,17 +3548,17 @@
         <v>62.5</v>
       </c>
     </row>
-    <row r="7" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B7" s="10" t="s">
+    <row r="7" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B7" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
+      <c r="C7" s="13"/>
+      <c r="D7" s="13"/>
+      <c r="E7" s="13"/>
+      <c r="F7" s="13"/>
+      <c r="G7" s="13"/>
     </row>
-    <row r="8" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B8" s="1" t="s">
         <v>0</v>
       </c>
@@ -3578,7 +3578,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B9" s="2">
         <v>1</v>
       </c>
@@ -3603,10 +3603,10 @@
         <v>1</v>
       </c>
       <c r="H9" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
-    <row r="10" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B10" s="2">
         <v>2</v>
       </c>
@@ -3631,7 +3631,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B11" s="2" t="s">
         <v>8</v>
       </c>
@@ -3653,23 +3653,23 @@
       </c>
       <c r="G11" s="4"/>
       <c r="H11" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="S11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B13" s="10" t="s">
+    <row r="13" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B13" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
+      <c r="C13" s="13"/>
+      <c r="D13" s="13"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
       <c r="G13" s="7"/>
     </row>
-    <row r="14" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B14" s="1" t="s">
         <v>0</v>
       </c>
@@ -3685,9 +3685,9 @@
       <c r="F14" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G14" s="12"/>
+      <c r="G14" s="10"/>
     </row>
-    <row r="15" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B15" s="2">
         <v>1</v>
       </c>
@@ -3707,11 +3707,11 @@
         <f t="shared" si="3"/>
         <v>50</v>
       </c>
-      <c r="G15" s="13" t="s">
-        <v>18</v>
+      <c r="G15" s="11" t="s">
+        <v>21</v>
       </c>
     </row>
-    <row r="16" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B16" s="2">
         <v>2</v>
       </c>
@@ -3731,22 +3731,22 @@
         <f t="shared" si="4"/>
         <v>62.5</v>
       </c>
-      <c r="G16" s="13"/>
+      <c r="G16" s="11"/>
     </row>
-    <row r="17" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="G17" s="14"/>
+    <row r="17" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="G17" s="12"/>
     </row>
-    <row r="18" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B18" s="11" t="s">
+    <row r="18" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B18" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C18" s="11"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="11"/>
-      <c r="F18" s="11"/>
-      <c r="G18" s="14"/>
+      <c r="C18" s="14"/>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+      <c r="G18" s="12"/>
     </row>
-    <row r="19" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B19" s="1" t="s">
         <v>0</v>
       </c>
@@ -3762,9 +3762,9 @@
       <c r="F19" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G19" s="14"/>
+      <c r="G19" s="12"/>
     </row>
-    <row r="20" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B20" s="2">
         <v>3</v>
       </c>
@@ -3784,36 +3784,36 @@
         <f>1.8398*12+47.8</f>
         <v>69.877600000000001</v>
       </c>
-      <c r="G20" s="14" t="s">
-        <v>21</v>
+      <c r="G20" s="12" t="s">
+        <v>18</v>
       </c>
     </row>
-    <row r="21" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="G21" s="14" t="s">
-        <v>19</v>
+    <row r="21" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="G21" s="12" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="22" spans="2:19" x14ac:dyDescent="0.3">
-      <c r="B22" s="11" t="s">
+    <row r="22" spans="2:19" x14ac:dyDescent="0.35">
+      <c r="B22" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11"/>
-      <c r="E22" s="11"/>
-      <c r="F22" s="11"/>
-      <c r="G22" s="14"/>
-      <c r="K22" s="10" t="s">
+      <c r="C22" s="14"/>
+      <c r="D22" s="14"/>
+      <c r="E22" s="14"/>
+      <c r="F22" s="14"/>
+      <c r="G22" s="12"/>
+      <c r="K22" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="L22" s="10"/>
-      <c r="M22" s="10"/>
-      <c r="N22" s="10"/>
-      <c r="O22" s="10"/>
-      <c r="P22" s="10"/>
-      <c r="Q22" s="10"/>
-      <c r="R22" s="10"/>
+      <c r="L22" s="13"/>
+      <c r="M22" s="13"/>
+      <c r="N22" s="13"/>
+      <c r="O22" s="13"/>
+      <c r="P22" s="13"/>
+      <c r="Q22" s="13"/>
+      <c r="R22" s="13"/>
     </row>
-    <row r="23" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B23" s="1" t="s">
         <v>0</v>
       </c>
@@ -3829,7 +3829,7 @@
       <c r="F23" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G23" s="14"/>
+      <c r="G23" s="12"/>
       <c r="K23" s="1" t="s">
         <v>1</v>
       </c>
@@ -3855,7 +3855,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B24" s="2">
         <v>3</v>
       </c>
@@ -3875,8 +3875,8 @@
         <f t="shared" si="5"/>
         <v>111.80416000000001</v>
       </c>
-      <c r="G24" s="14" t="s">
-        <v>20</v>
+      <c r="G24" s="12" t="s">
+        <v>17</v>
       </c>
       <c r="K24" s="2">
         <v>50</v>
@@ -3903,56 +3903,56 @@
         <v>62.5</v>
       </c>
     </row>
-    <row r="25" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B25" s="9"/>
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
       <c r="E25" s="9"/>
       <c r="F25" s="9"/>
     </row>
-    <row r="26" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B26" s="7"/>
       <c r="C26" s="7"/>
       <c r="D26" s="7"/>
       <c r="E26" s="7"/>
       <c r="F26" s="7"/>
     </row>
-    <row r="27" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B27" s="6"/>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>
       <c r="F27" s="6"/>
     </row>
-    <row r="28" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:19" x14ac:dyDescent="0.35">
       <c r="B28" s="6"/>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
       <c r="E28" s="8"/>
       <c r="F28" s="8"/>
     </row>
-    <row r="29" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:19" x14ac:dyDescent="0.35">
       <c r="S29" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="43" spans="11:22" x14ac:dyDescent="0.3">
-      <c r="K43" s="10" t="s">
+    <row r="43" spans="11:22" x14ac:dyDescent="0.35">
+      <c r="K43" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="L43" s="10"/>
-      <c r="M43" s="10"/>
-      <c r="N43" s="10"/>
-      <c r="O43" s="10"/>
-      <c r="P43" s="10"/>
-      <c r="Q43" s="10"/>
-      <c r="R43" s="10"/>
-      <c r="S43" s="10"/>
-      <c r="T43" s="10"/>
-      <c r="U43" s="10"/>
-      <c r="V43" s="10"/>
+      <c r="L43" s="13"/>
+      <c r="M43" s="13"/>
+      <c r="N43" s="13"/>
+      <c r="O43" s="13"/>
+      <c r="P43" s="13"/>
+      <c r="Q43" s="13"/>
+      <c r="R43" s="13"/>
+      <c r="S43" s="13"/>
+      <c r="T43" s="13"/>
+      <c r="U43" s="13"/>
+      <c r="V43" s="13"/>
     </row>
-    <row r="44" spans="11:22" x14ac:dyDescent="0.3">
+    <row r="44" spans="11:22" x14ac:dyDescent="0.35">
       <c r="K44" s="1" t="s">
         <v>1</v>
       </c>
@@ -3990,7 +3990,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="11:22" x14ac:dyDescent="0.3">
+    <row r="45" spans="11:22" x14ac:dyDescent="0.35">
       <c r="K45" s="2">
         <v>40</v>
       </c>
@@ -4028,7 +4028,7 @@
         <v>111.80416000000001</v>
       </c>
     </row>
-    <row r="52" spans="19:19" x14ac:dyDescent="0.3">
+    <row r="52" spans="19:19" x14ac:dyDescent="0.35">
       <c r="S52" t="s">
         <v>11</v>
       </c>

</xml_diff>